<commit_message>
added some missing fields
</commit_message>
<xml_diff>
--- a/django_project/wfrp/example_media/initial_characters.xlsx
+++ b/django_project/wfrp/example_media/initial_characters.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -169,7 +169,7 @@
     <t xml:space="preserve">consume_alcohol</t>
   </si>
   <si>
-    <t xml:space="preserve"> dodge</t>
+    <t xml:space="preserve">dodge</t>
   </si>
   <si>
     <t xml:space="preserve">drive</t>
@@ -257,6 +257,12 @@
   </si>
   <si>
     <t xml:space="preserve">body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_wounds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heal</t>
   </si>
   <si>
     <t xml:space="preserve">Gunnar Hrolfsson</t>
@@ -343,6 +349,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -364,6 +371,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -440,19 +448,19 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T4" activeCellId="0" sqref="T4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BK1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CC6" activeCellId="0" sqref="CC6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="82.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="33.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="60.16"/>
@@ -460,7 +468,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="21.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="21.56"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,29 +709,35 @@
       <c r="CA1" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="CB1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="2" customFormat="true" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>59</v>
@@ -732,40 +746,40 @@
         <v>4.8</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="W2" s="2" t="n">
         <v>45</v>
@@ -900,19 +914,19 @@
         <v>23</v>
       </c>
       <c r="BO2" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="BP2" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="BQ2" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="BR2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="BS2" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="BT2" s="2" t="n">
         <v>200</v>
@@ -937,6 +951,12 @@
       </c>
       <c r="CA2" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="CB2" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="CC2" s="2" t="n">
+        <v>38</v>
       </c>
       <c r="AMJ2" s="0"/>
     </row>

</xml_diff>

<commit_message>
implemented models for missing character sheet entities
</commit_message>
<xml_diff>
--- a/django_project/wfrp/example_media/initial_characters.xlsx
+++ b/django_project/wfrp/example_media/initial_characters.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -235,9 +235,6 @@
     <t xml:space="preserve">mutations</t>
   </si>
   <si>
-    <t xml:space="preserve">wealth</t>
-  </si>
-  <si>
     <t xml:space="preserve">wounds</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
   </si>
   <si>
     <t xml:space="preserve">max_wounds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">heal</t>
   </si>
   <si>
     <t xml:space="preserve">Gunnar Hrolfsson</t>
@@ -449,10 +443,10 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BK1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CC6" activeCellId="0" sqref="CC6"/>
+      <selection pane="topLeft" activeCell="BT1" activeCellId="0" sqref="BT1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.39"/>
@@ -469,6 +463,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,35 +704,31 @@
       <c r="CA1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="2" customFormat="true" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>59</v>
@@ -746,40 +737,40 @@
         <v>4.8</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="W2" s="2" t="n">
         <v>45</v>
@@ -914,25 +905,25 @@
         <v>23</v>
       </c>
       <c r="BO2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="BP2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="BQ2" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="BR2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="BS2" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="BT2" s="2" t="n">
-        <v>200</v>
+        <v>18</v>
       </c>
       <c r="BU2" s="2" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="BV2" s="2" t="n">
         <v>0</v>
@@ -950,14 +941,10 @@
         <v>0</v>
       </c>
       <c r="CA2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="CB2" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="CC2" s="2" t="n">
-        <v>38</v>
-      </c>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
   </sheetData>

</xml_diff>